<commit_message>
Pet data driven Test cases
</commit_message>
<xml_diff>
--- a/testdata/testdata.xlsx
+++ b/testdata/testdata.xlsx
@@ -5,36 +5,28 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1666db94a1cb56fd/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hari\eclipse-workspace\RestAssuredProject\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5168FD5-AE77-4A00-B363-1F4FD0E4313C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17BFD662-54F6-4977-A00D-449C26284205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{18636C25-6CF3-4A74-A46A-06B53D3CC068}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{18636C25-6CF3-4A74-A46A-06B53D3CC068}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="USER" sheetId="1" r:id="rId1"/>
+    <sheet name="PET" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
   <si>
     <t>ID</t>
   </si>
@@ -142,6 +134,72 @@
   </si>
   <si>
     <t>test@6</t>
+  </si>
+  <si>
+    <t>PETID</t>
+  </si>
+  <si>
+    <t>CID</t>
+  </si>
+  <si>
+    <t>CNAME</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>PHOTOURL</t>
+  </si>
+  <si>
+    <t>TID</t>
+  </si>
+  <si>
+    <t>TNAME</t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>dog</t>
+  </si>
+  <si>
+    <t>doggie</t>
+  </si>
+  <si>
+    <t>https://www.shutterstock.com/image-photo/parrot-on-branch-260nw-714651400.jpg</t>
+  </si>
+  <si>
+    <t>available</t>
+  </si>
+  <si>
+    <t>cat</t>
+  </si>
+  <si>
+    <t>cattie</t>
+  </si>
+  <si>
+    <t>monkey</t>
+  </si>
+  <si>
+    <t>monkeynkeyie</t>
+  </si>
+  <si>
+    <t>rino</t>
+  </si>
+  <si>
+    <t>rinonoie</t>
+  </si>
+  <si>
+    <t>cocktail</t>
+  </si>
+  <si>
+    <t>cocktailcktailie</t>
+  </si>
+  <si>
+    <t>parrot</t>
+  </si>
+  <si>
+    <t>parrotrrotie</t>
   </si>
 </sst>
 </file>
@@ -206,12 +264,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -529,7 +590,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26429FB5-6503-416D-899D-73CA55B70670}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -719,4 +780,208 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88AEEE5B-5209-4813-ADD6-5FC8D7AA47BC}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="17.7265625" customWidth="1"/>
+    <col min="5" max="5" width="16.90625" customWidth="1"/>
+    <col min="6" max="6" width="9.54296875" customWidth="1"/>
+    <col min="7" max="7" width="10.26953125" customWidth="1"/>
+    <col min="8" max="8" width="19.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>101</v>
+      </c>
+      <c r="B2">
+        <v>1011</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2">
+        <v>1011</v>
+      </c>
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>102</v>
+      </c>
+      <c r="B3">
+        <v>1022</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3">
+        <v>1022</v>
+      </c>
+      <c r="G3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>103</v>
+      </c>
+      <c r="B4">
+        <v>1033</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4">
+        <v>1033</v>
+      </c>
+      <c r="G4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>104</v>
+      </c>
+      <c r="B5">
+        <v>1044</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5">
+        <v>1044</v>
+      </c>
+      <c r="G5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>105</v>
+      </c>
+      <c r="B6">
+        <v>1055</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6">
+        <v>1055</v>
+      </c>
+      <c r="G6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>106</v>
+      </c>
+      <c r="B7">
+        <v>1066</v>
+      </c>
+      <c r="C7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7">
+        <v>1066</v>
+      </c>
+      <c r="G7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>